<commit_message>
Set Golf non-majors men payouts to dash pending official confirmation
</commit_message>
<xml_diff>
--- a/Winnings.xlsx
+++ b/Winnings.xlsx
@@ -5759,351 +5759,351 @@
         <v>Finish</v>
       </c>
       <c r="B160" t="str">
-        <v>The Players Championship($25M)</v>
+        <v>The Players Championship</v>
       </c>
       <c r="C160" t="str">
-        <v>AT&amp;T Pebble Beach Pro-Am($20M)</v>
+        <v>AT&amp;T Pebble Beach Pro-Am</v>
       </c>
       <c r="D160" t="str">
-        <v>Genesis Invitational($20M)</v>
+        <v>Genesis Invitational</v>
       </c>
       <c r="E160" t="str">
-        <v>Arnold Palmer Invitational($20M)</v>
+        <v>Arnold Palmer Invitational</v>
       </c>
       <c r="F160" t="str">
-        <v>RBC Heritage($20M)</v>
+        <v>RBC Heritage</v>
       </c>
       <c r="G160" t="str">
-        <v>Memorial Tournament($20M)</v>
+        <v>Memorial Tournament</v>
       </c>
       <c r="H160" t="str">
-        <v>Travelers Championship($20M)</v>
+        <v>Travelers Championship</v>
       </c>
       <c r="I160" t="str">
-        <v>FedEx St. Jude Championship($20M)</v>
+        <v>FedEx St. Jude Championship</v>
       </c>
       <c r="J160" t="str">
-        <v>BMW Championship($20M)</v>
+        <v>BMW Championship</v>
       </c>
     </row>
     <row r="161">
       <c r="A161">
         <v>1</v>
       </c>
-      <c r="B161">
-        <v>4500000</v>
-      </c>
-      <c r="C161">
-        <v>3600000</v>
-      </c>
-      <c r="D161">
-        <v>4000000</v>
-      </c>
-      <c r="E161">
-        <v>4000000</v>
-      </c>
-      <c r="F161">
-        <v>3600000</v>
-      </c>
-      <c r="G161">
-        <v>4000000</v>
-      </c>
-      <c r="H161">
-        <v>3600000</v>
-      </c>
-      <c r="I161">
-        <v>3600000</v>
-      </c>
-      <c r="J161">
-        <v>3600000</v>
+      <c r="B161" t="str">
+        <v>-</v>
+      </c>
+      <c r="C161" t="str">
+        <v>-</v>
+      </c>
+      <c r="D161" t="str">
+        <v>-</v>
+      </c>
+      <c r="E161" t="str">
+        <v>-</v>
+      </c>
+      <c r="F161" t="str">
+        <v>-</v>
+      </c>
+      <c r="G161" t="str">
+        <v>-</v>
+      </c>
+      <c r="H161" t="str">
+        <v>-</v>
+      </c>
+      <c r="I161" t="str">
+        <v>-</v>
+      </c>
+      <c r="J161" t="str">
+        <v>-</v>
       </c>
     </row>
     <row r="162">
       <c r="A162">
         <v>2</v>
       </c>
-      <c r="B162">
-        <v>2725000</v>
-      </c>
-      <c r="C162">
-        <v>2160000</v>
-      </c>
-      <c r="D162">
-        <v>2200000</v>
-      </c>
-      <c r="E162">
-        <v>2200000</v>
-      </c>
-      <c r="F162">
-        <v>2160000</v>
-      </c>
-      <c r="G162">
-        <v>2200000</v>
-      </c>
-      <c r="H162">
-        <v>2160000</v>
-      </c>
-      <c r="I162">
-        <v>2160000</v>
-      </c>
-      <c r="J162">
-        <v>2160000</v>
+      <c r="B162" t="str">
+        <v>-</v>
+      </c>
+      <c r="C162" t="str">
+        <v>-</v>
+      </c>
+      <c r="D162" t="str">
+        <v>-</v>
+      </c>
+      <c r="E162" t="str">
+        <v>-</v>
+      </c>
+      <c r="F162" t="str">
+        <v>-</v>
+      </c>
+      <c r="G162" t="str">
+        <v>-</v>
+      </c>
+      <c r="H162" t="str">
+        <v>-</v>
+      </c>
+      <c r="I162" t="str">
+        <v>-</v>
+      </c>
+      <c r="J162" t="str">
+        <v>-</v>
       </c>
     </row>
     <row r="163">
       <c r="A163">
         <v>3</v>
       </c>
-      <c r="B163">
-        <v>1725000</v>
-      </c>
-      <c r="C163">
-        <v>1360000</v>
-      </c>
-      <c r="D163">
-        <v>1400000</v>
-      </c>
-      <c r="E163">
-        <v>1400000</v>
-      </c>
-      <c r="F163">
-        <v>1360000</v>
-      </c>
-      <c r="G163">
-        <v>1400000</v>
-      </c>
-      <c r="H163">
-        <v>1360000</v>
-      </c>
-      <c r="I163">
-        <v>1360000</v>
-      </c>
-      <c r="J163">
-        <v>1360000</v>
+      <c r="B163" t="str">
+        <v>-</v>
+      </c>
+      <c r="C163" t="str">
+        <v>-</v>
+      </c>
+      <c r="D163" t="str">
+        <v>-</v>
+      </c>
+      <c r="E163" t="str">
+        <v>-</v>
+      </c>
+      <c r="F163" t="str">
+        <v>-</v>
+      </c>
+      <c r="G163" t="str">
+        <v>-</v>
+      </c>
+      <c r="H163" t="str">
+        <v>-</v>
+      </c>
+      <c r="I163" t="str">
+        <v>-</v>
+      </c>
+      <c r="J163" t="str">
+        <v>-</v>
       </c>
     </row>
     <row r="164">
       <c r="A164">
         <v>4</v>
       </c>
-      <c r="B164">
-        <v>1225000</v>
-      </c>
-      <c r="C164">
-        <v>960000</v>
-      </c>
-      <c r="D164">
-        <v>1000000</v>
-      </c>
-      <c r="E164">
-        <v>1000000</v>
-      </c>
-      <c r="F164">
-        <v>960000</v>
-      </c>
-      <c r="G164">
-        <v>1000000</v>
-      </c>
-      <c r="H164">
-        <v>960000</v>
-      </c>
-      <c r="I164">
-        <v>960000</v>
-      </c>
-      <c r="J164">
-        <v>960000</v>
+      <c r="B164" t="str">
+        <v>-</v>
+      </c>
+      <c r="C164" t="str">
+        <v>-</v>
+      </c>
+      <c r="D164" t="str">
+        <v>-</v>
+      </c>
+      <c r="E164" t="str">
+        <v>-</v>
+      </c>
+      <c r="F164" t="str">
+        <v>-</v>
+      </c>
+      <c r="G164" t="str">
+        <v>-</v>
+      </c>
+      <c r="H164" t="str">
+        <v>-</v>
+      </c>
+      <c r="I164" t="str">
+        <v>-</v>
+      </c>
+      <c r="J164" t="str">
+        <v>-</v>
       </c>
     </row>
     <row r="165">
       <c r="A165">
         <v>5</v>
       </c>
-      <c r="B165">
-        <v>1025000</v>
-      </c>
-      <c r="C165">
-        <v>800000</v>
-      </c>
-      <c r="D165">
-        <v>840000</v>
-      </c>
-      <c r="E165">
-        <v>840000</v>
-      </c>
-      <c r="F165">
-        <v>800000</v>
-      </c>
-      <c r="G165">
-        <v>840000</v>
-      </c>
-      <c r="H165">
-        <v>800000</v>
-      </c>
-      <c r="I165">
-        <v>800000</v>
-      </c>
-      <c r="J165">
-        <v>800000</v>
+      <c r="B165" t="str">
+        <v>-</v>
+      </c>
+      <c r="C165" t="str">
+        <v>-</v>
+      </c>
+      <c r="D165" t="str">
+        <v>-</v>
+      </c>
+      <c r="E165" t="str">
+        <v>-</v>
+      </c>
+      <c r="F165" t="str">
+        <v>-</v>
+      </c>
+      <c r="G165" t="str">
+        <v>-</v>
+      </c>
+      <c r="H165" t="str">
+        <v>-</v>
+      </c>
+      <c r="I165" t="str">
+        <v>-</v>
+      </c>
+      <c r="J165" t="str">
+        <v>-</v>
       </c>
     </row>
     <row r="166">
       <c r="A166">
         <v>6</v>
       </c>
-      <c r="B166">
-        <v>906250</v>
-      </c>
-      <c r="C166">
-        <v>720000</v>
-      </c>
-      <c r="D166">
-        <v>760000</v>
-      </c>
-      <c r="E166">
-        <v>760000</v>
-      </c>
-      <c r="F166">
-        <v>720000</v>
-      </c>
-      <c r="G166">
-        <v>760000</v>
-      </c>
-      <c r="H166">
-        <v>720000</v>
-      </c>
-      <c r="I166">
-        <v>720000</v>
-      </c>
-      <c r="J166">
-        <v>720000</v>
+      <c r="B166" t="str">
+        <v>-</v>
+      </c>
+      <c r="C166" t="str">
+        <v>-</v>
+      </c>
+      <c r="D166" t="str">
+        <v>-</v>
+      </c>
+      <c r="E166" t="str">
+        <v>-</v>
+      </c>
+      <c r="F166" t="str">
+        <v>-</v>
+      </c>
+      <c r="G166" t="str">
+        <v>-</v>
+      </c>
+      <c r="H166" t="str">
+        <v>-</v>
+      </c>
+      <c r="I166" t="str">
+        <v>-</v>
+      </c>
+      <c r="J166" t="str">
+        <v>-</v>
       </c>
     </row>
     <row r="167">
       <c r="A167">
         <v>7</v>
       </c>
-      <c r="B167">
-        <v>843750</v>
-      </c>
-      <c r="C167">
-        <v>670000</v>
-      </c>
-      <c r="D167">
-        <v>700000</v>
-      </c>
-      <c r="E167">
-        <v>700000</v>
-      </c>
-      <c r="F167">
-        <v>670000</v>
-      </c>
-      <c r="G167">
-        <v>700000</v>
-      </c>
-      <c r="H167">
-        <v>670000</v>
-      </c>
-      <c r="I167">
-        <v>670000</v>
-      </c>
-      <c r="J167">
-        <v>670000</v>
+      <c r="B167" t="str">
+        <v>-</v>
+      </c>
+      <c r="C167" t="str">
+        <v>-</v>
+      </c>
+      <c r="D167" t="str">
+        <v>-</v>
+      </c>
+      <c r="E167" t="str">
+        <v>-</v>
+      </c>
+      <c r="F167" t="str">
+        <v>-</v>
+      </c>
+      <c r="G167" t="str">
+        <v>-</v>
+      </c>
+      <c r="H167" t="str">
+        <v>-</v>
+      </c>
+      <c r="I167" t="str">
+        <v>-</v>
+      </c>
+      <c r="J167" t="str">
+        <v>-</v>
       </c>
     </row>
     <row r="168">
       <c r="A168">
         <v>8</v>
       </c>
-      <c r="B168">
-        <v>781250</v>
-      </c>
-      <c r="C168">
-        <v>620000</v>
-      </c>
-      <c r="D168">
-        <v>650000</v>
-      </c>
-      <c r="E168">
-        <v>650000</v>
-      </c>
-      <c r="F168">
-        <v>620000</v>
-      </c>
-      <c r="G168">
-        <v>650000</v>
-      </c>
-      <c r="H168">
-        <v>620000</v>
-      </c>
-      <c r="I168">
-        <v>620000</v>
-      </c>
-      <c r="J168">
-        <v>620000</v>
+      <c r="B168" t="str">
+        <v>-</v>
+      </c>
+      <c r="C168" t="str">
+        <v>-</v>
+      </c>
+      <c r="D168" t="str">
+        <v>-</v>
+      </c>
+      <c r="E168" t="str">
+        <v>-</v>
+      </c>
+      <c r="F168" t="str">
+        <v>-</v>
+      </c>
+      <c r="G168" t="str">
+        <v>-</v>
+      </c>
+      <c r="H168" t="str">
+        <v>-</v>
+      </c>
+      <c r="I168" t="str">
+        <v>-</v>
+      </c>
+      <c r="J168" t="str">
+        <v>-</v>
       </c>
     </row>
     <row r="169">
       <c r="A169">
         <v>9</v>
       </c>
-      <c r="B169">
-        <v>731250</v>
-      </c>
-      <c r="C169">
-        <v>580000</v>
-      </c>
-      <c r="D169">
-        <v>610000</v>
-      </c>
-      <c r="E169">
-        <v>610000</v>
-      </c>
-      <c r="F169">
-        <v>580000</v>
-      </c>
-      <c r="G169">
-        <v>610000</v>
-      </c>
-      <c r="H169">
-        <v>580000</v>
-      </c>
-      <c r="I169">
-        <v>580000</v>
-      </c>
-      <c r="J169">
-        <v>580000</v>
+      <c r="B169" t="str">
+        <v>-</v>
+      </c>
+      <c r="C169" t="str">
+        <v>-</v>
+      </c>
+      <c r="D169" t="str">
+        <v>-</v>
+      </c>
+      <c r="E169" t="str">
+        <v>-</v>
+      </c>
+      <c r="F169" t="str">
+        <v>-</v>
+      </c>
+      <c r="G169" t="str">
+        <v>-</v>
+      </c>
+      <c r="H169" t="str">
+        <v>-</v>
+      </c>
+      <c r="I169" t="str">
+        <v>-</v>
+      </c>
+      <c r="J169" t="str">
+        <v>-</v>
       </c>
     </row>
     <row r="170">
       <c r="A170">
         <v>10</v>
       </c>
-      <c r="B170">
-        <v>681250</v>
-      </c>
-      <c r="C170">
-        <v>540000</v>
-      </c>
-      <c r="D170">
-        <v>570000</v>
-      </c>
-      <c r="E170">
-        <v>570000</v>
-      </c>
-      <c r="F170">
-        <v>540000</v>
-      </c>
-      <c r="G170">
-        <v>570000</v>
-      </c>
-      <c r="H170">
-        <v>540000</v>
-      </c>
-      <c r="I170">
-        <v>540000</v>
-      </c>
-      <c r="J170">
-        <v>540000</v>
+      <c r="B170" t="str">
+        <v>-</v>
+      </c>
+      <c r="C170" t="str">
+        <v>-</v>
+      </c>
+      <c r="D170" t="str">
+        <v>-</v>
+      </c>
+      <c r="E170" t="str">
+        <v>-</v>
+      </c>
+      <c r="F170" t="str">
+        <v>-</v>
+      </c>
+      <c r="G170" t="str">
+        <v>-</v>
+      </c>
+      <c r="H170" t="str">
+        <v>-</v>
+      </c>
+      <c r="I170" t="str">
+        <v>-</v>
+      </c>
+      <c r="J170" t="str">
+        <v>-</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fill official non-majors men winner payouts and keep others dashed
</commit_message>
<xml_diff>
--- a/Winnings.xlsx
+++ b/Winnings.xlsx
@@ -5790,32 +5790,32 @@
       <c r="A161">
         <v>1</v>
       </c>
-      <c r="B161" t="str">
-        <v>-</v>
-      </c>
-      <c r="C161" t="str">
-        <v>-</v>
-      </c>
-      <c r="D161" t="str">
-        <v>-</v>
-      </c>
-      <c r="E161" t="str">
-        <v>-</v>
-      </c>
-      <c r="F161" t="str">
-        <v>-</v>
-      </c>
-      <c r="G161" t="str">
-        <v>-</v>
-      </c>
-      <c r="H161" t="str">
-        <v>-</v>
-      </c>
-      <c r="I161" t="str">
-        <v>-</v>
-      </c>
-      <c r="J161" t="str">
-        <v>-</v>
+      <c r="B161">
+        <v>4500000</v>
+      </c>
+      <c r="C161">
+        <v>3600000</v>
+      </c>
+      <c r="D161">
+        <v>4000000</v>
+      </c>
+      <c r="E161">
+        <v>4000000</v>
+      </c>
+      <c r="F161">
+        <v>3600000</v>
+      </c>
+      <c r="G161">
+        <v>4000000</v>
+      </c>
+      <c r="H161">
+        <v>3600000</v>
+      </c>
+      <c r="I161">
+        <v>3600000</v>
+      </c>
+      <c r="J161">
+        <v>3600000</v>
       </c>
     </row>
     <row r="162">

</xml_diff>